<commit_message>
Addew new hubs to the list
</commit_message>
<xml_diff>
--- a/data/20210219_innovation_hubs-Almasi-v1.xlsx
+++ b/data/20210219_innovation_hubs-Almasi-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sirvan/sites/startups/psychi/innovation-hubs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58084A9B-3FDC-654E-A607-C8C27AC9F79D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B260D-8228-8E47-BDA6-76BC94977EC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="619">
   <si>
     <t>Google Campus London</t>
   </si>
@@ -1849,13 +1849,55 @@
   </si>
   <si>
     <t>University of Gloucestershire;The Park;Cheltenham;GL50 2RH.</t>
+  </si>
+  <si>
+    <t>https://ktn-uk.org/programme/cyberasap/</t>
+  </si>
+  <si>
+    <t>CyberASAP</t>
+  </si>
+  <si>
+    <t>Pre-seed</t>
+  </si>
+  <si>
+    <t>CyberASAP is funded by the UK Government Department for Digital, Culture Media &amp; Sport (DCMS) and delivered through KTN and Innovate UK.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Digital Catapult</t>
+  </si>
+  <si>
+    <t>https://www.digicatapult.org.uk/</t>
+  </si>
+  <si>
+    <t>info@digicatapult.org.uk</t>
+  </si>
+  <si>
+    <t>Hub</t>
+  </si>
+  <si>
+    <t>101 Euston Road; London; NW1 2RA</t>
+  </si>
+  <si>
+    <t>AI; VR; AR; IoT; 5G</t>
+  </si>
+  <si>
+    <t>London; Endinbugh</t>
+  </si>
+  <si>
+    <t>Accelerating early adoption of advanced digital technology. Digital Catapult specialises in Future Networks, AI and Immersive.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1884,6 +1926,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1902,10 +1952,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1917,8 +1968,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2255,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G147"/>
+  <dimension ref="A1:H149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2272,7 +2327,7 @@
     <col min="8" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>469</v>
       </c>
@@ -2292,8 +2347,11 @@
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -2312,8 +2370,11 @@
         <v>470</v>
       </c>
       <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -2333,7 +2394,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>473</v>
       </c>
@@ -2355,7 +2416,7 @@
       </c>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -2375,7 +2436,7 @@
       </c>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -2399,7 +2460,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>17</v>
@@ -2419,7 +2480,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>19</v>
@@ -2441,7 +2502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>22</v>
@@ -2463,7 +2524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>27</v>
@@ -2483,7 +2544,7 @@
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>29</v>
@@ -2505,7 +2566,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>34</v>
@@ -2527,7 +2588,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>38</v>
@@ -2547,7 +2608,7 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>40</v>
@@ -2569,7 +2630,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" t="s">
         <v>44</v>
@@ -2591,7 +2652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" t="s">
         <v>48</v>
@@ -5112,7 +5173,7 @@
         <v>408</v>
       </c>
       <c r="D131" t="str">
-        <f t="shared" ref="D131:D147" si="2">CONCATENATE("* [",B131,"](",C131,")")</f>
+        <f t="shared" ref="D131:D149" si="2">CONCATENATE("* [",B131,"](",C131,")")</f>
         <v>* [Londoneast](https://www.londoneast-uk.com/)</v>
       </c>
       <c r="E131" t="s">
@@ -5411,7 +5472,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145"/>
       <c r="B145" t="s">
         <v>449</v>
@@ -5433,7 +5494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146"/>
       <c r="B146" t="s">
         <v>452</v>
@@ -5455,7 +5516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147"/>
       <c r="B147" t="s">
         <v>455</v>
@@ -5477,9 +5538,66 @@
         <v>54</v>
       </c>
     </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="2"/>
+        <v>* [CyberASAP](https://ktn-uk.org/programme/cyberasap/)</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G148" t="s">
+        <v>54</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Digital Catapult](https://www.digicatapult.org.uk/)</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="G149" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G149" r:id="rId1" xr:uid="{5DEB78D7-D928-2C42-A7E2-04D9DE29B9C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the big names
</commit_message>
<xml_diff>
--- a/data/20210219_innovation_hubs-Almasi-v1.xlsx
+++ b/data/20210219_innovation_hubs-Almasi-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sirvan/sites/startups/psychi/innovation-hubs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B260D-8228-8E47-BDA6-76BC94977EC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1236063-1601-2940-8AC3-5C4A4CA247D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="647">
   <si>
     <t>Google Campus London</t>
   </si>
@@ -1887,10 +1887,94 @@
     <t>AI; VR; AR; IoT; 5G</t>
   </si>
   <si>
-    <t>London; Endinbugh</t>
-  </si>
-  <si>
     <t>Accelerating early adoption of advanced digital technology. Digital Catapult specialises in Future Networks, AI and Immersive.</t>
+  </si>
+  <si>
+    <t>ktn</t>
+  </si>
+  <si>
+    <t>Hub; Gov; Fund; Accelerator</t>
+  </si>
+  <si>
+    <t>https://ktn-uk.org/</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>KTNUK</t>
+  </si>
+  <si>
+    <t>London; Endinbugh; Oxford</t>
+  </si>
+  <si>
+    <t>London (N1 0QH); Endinbugh (EH2 2PJ); Oxford (OX11 0GD)</t>
+  </si>
+  <si>
+    <t>(+44) 03333 403250</t>
+  </si>
+  <si>
+    <t>Gov; Fund</t>
+  </si>
+  <si>
+    <t>innovateuk</t>
+  </si>
+  <si>
+    <t>UK’s Innovation agency. We fund business &amp; research collaborations to accelerate innovation &amp; drive business</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/organisations/innovate-uk</t>
+  </si>
+  <si>
+    <t>https://www.ukri.org/</t>
+  </si>
+  <si>
+    <t>UK Research and Innovation (UKRI)</t>
+  </si>
+  <si>
+    <t>Innovate UK (part of UKRI)</t>
+  </si>
+  <si>
+    <t>Polaris House; North Star Avenue; Swindon; Wiltshire; SN2 1FL</t>
+  </si>
+  <si>
+    <t>UKRI_News</t>
+  </si>
+  <si>
+    <t>UK Research and Innovation (UKRI) is the national funding agency investing in science and research in the UK. Operating across the whole of the UK with a combined budget of more than £6 billion, UKRI brings together the 7 Research Councils, Innovate UK and Research England.</t>
+  </si>
+  <si>
+    <t>58 Victoria Embankment; London; EC4Y 0DS</t>
+  </si>
+  <si>
+    <t>Nicholson House; Lime Kiln Close; Stoke Gifford; Bristol; BS34 8SR</t>
+  </si>
+  <si>
+    <t>UKRI London Office</t>
+  </si>
+  <si>
+    <t>UKRI Bristol Office</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>UK Business Angels</t>
+  </si>
+  <si>
+    <t>https://www.ukbaa.org.uk/</t>
+  </si>
+  <si>
+    <t>Chancery House; Chancery Lane; London; WC2A 1QS</t>
+  </si>
+  <si>
+    <t>enquiries@ukbaa.org.uk</t>
+  </si>
+  <si>
+    <t>UKBAngels</t>
+  </si>
+  <si>
+    <t>The Trade Body for Angel and Early Stage Investing.</t>
   </si>
 </sst>
 </file>
@@ -2310,15 +2394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" style="2" customWidth="1"/>
     <col min="3" max="4" width="44.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -2327,7 +2411,7 @@
     <col min="8" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>469</v>
       </c>
@@ -2350,8 +2434,11 @@
       <c r="H1" s="1" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -2374,7 +2461,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -2394,7 +2481,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>473</v>
       </c>
@@ -2416,7 +2503,7 @@
       </c>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -2436,7 +2523,7 @@
       </c>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -2460,7 +2547,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>17</v>
@@ -2480,7 +2567,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>19</v>
@@ -2502,7 +2589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>22</v>
@@ -2524,7 +2611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>27</v>
@@ -2544,7 +2631,7 @@
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>29</v>
@@ -2566,7 +2653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>34</v>
@@ -2588,7 +2675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>38</v>
@@ -2608,7 +2695,7 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>40</v>
@@ -2630,7 +2717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" t="s">
         <v>44</v>
@@ -2652,7 +2739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" t="s">
         <v>48</v>
@@ -5173,7 +5260,7 @@
         <v>408</v>
       </c>
       <c r="D131" t="str">
-        <f t="shared" ref="D131:D149" si="2">CONCATENATE("* [",B131,"](",C131,")")</f>
+        <f t="shared" ref="D131:D155" si="2">CONCATENATE("* [",B131,"](",C131,")")</f>
         <v>* [Londoneast](https://www.londoneast-uk.com/)</v>
       </c>
       <c r="E131" t="s">
@@ -5472,7 +5559,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145"/>
       <c r="B145" t="s">
         <v>449</v>
@@ -5494,7 +5581,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146"/>
       <c r="B146" t="s">
         <v>452</v>
@@ -5516,7 +5603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147"/>
       <c r="B147" t="s">
         <v>455</v>
@@ -5538,7 +5625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>607</v>
       </c>
@@ -5556,7 +5643,7 @@
         <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="G148" t="s">
         <v>54</v>
@@ -5565,7 +5652,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>614</v>
       </c>
@@ -5589,15 +5676,199 @@
         <v>613</v>
       </c>
       <c r="H149" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>618</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D150" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [ktn](https://ktn-uk.org/)</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="D151" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Innovate UK (part of UKRI)](https://www.gov.uk/government/organisations/innovate-uk)</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G151" t="s">
+        <v>54</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="I151" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D152" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UK Research and Innovation (UKRI)](https://www.ukri.org/)</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G152" t="s">
+        <v>54</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I152" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D153" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UKRI London Office](https://www.ukri.org/)</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="G153" t="s">
+        <v>54</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D154" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UKRI Bristol Office](https://www.ukri.org/)</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="G154" t="s">
+        <v>54</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I154" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D155" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UK Business Angels](https://www.ukbaa.org.uk/)</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="G155" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="I155" s="2" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G149" r:id="rId1" xr:uid="{5DEB78D7-D928-2C42-A7E2-04D9DE29B9C3}"/>
+    <hyperlink ref="C150" r:id="rId2" xr:uid="{EBB988EE-9912-0949-ACEA-06FDF2FBFD29}"/>
+    <hyperlink ref="C151" r:id="rId3" xr:uid="{02B07F5C-084D-6C4A-BE49-66BE933E0C9C}"/>
+    <hyperlink ref="B152" r:id="rId4" display="https://www.ukri.org/" xr:uid="{916092C3-8665-F644-BBAF-0D339DA25E20}"/>
+    <hyperlink ref="B153" r:id="rId5" display="https://www.ukri.org/" xr:uid="{F71EA6AE-25FC-0643-B32F-0D7D1E7A3FFA}"/>
+    <hyperlink ref="B154" r:id="rId6" display="https://www.ukri.org/" xr:uid="{79805B14-AB51-844B-906C-76DB0A3D2308}"/>
+    <hyperlink ref="C155" r:id="rId7" xr:uid="{3662B43C-1CFF-6E45-B695-7DF9A558B0AC}"/>
+    <hyperlink ref="G155" r:id="rId8" xr:uid="{693D2C18-D32F-6043-81C1-485C2ADE2807}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Started to add an international tab
</commit_message>
<xml_diff>
--- a/data/20210219_innovation_hubs-Almasi-v1.xlsx
+++ b/data/20210219_innovation_hubs-Almasi-v1.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sirvan/sites/startups/psychi/innovation-hubs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0BC927-F300-C24E-883F-FA0386386232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316FEDAE-DE3A-F446-A9A3-26AAB95A9B99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33040" yWindow="2860" windowWidth="43800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="info" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="UK" sheetId="1" r:id="rId1"/>
+    <sheet name="US" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="659">
   <si>
     <t>Google Campus London</t>
   </si>
@@ -942,9 +941,6 @@
     <t>https://www.stevenagecatalyst.com/</t>
   </si>
   <si>
-    <t>Stevenage Bioscience Catalyst Gunnels Wood Road Stevenage Herts SG1 2FX</t>
-  </si>
-  <si>
     <t>comms@stevenagecatalyst.com</t>
   </si>
   <si>
@@ -2005,6 +2001,15 @@
   </si>
   <si>
     <t>Deeptech; life science; engineering; manufacturing</t>
+  </si>
+  <si>
+    <t>Stanford Digital Economy Lab</t>
+  </si>
+  <si>
+    <t>https://twitter.com/DigEconLab</t>
+  </si>
+  <si>
+    <t>Stevenage Bioscience Catalyst; Gunnels Wood Road; Stevenage Herts SG1 2FX</t>
   </si>
 </sst>
 </file>
@@ -2426,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2438,14 +2443,14 @@
     <col min="5" max="5" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="2"/>
+    <col min="8" max="8" width="13.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -2455,7 +2460,7 @@
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
@@ -2464,15 +2469,15 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2488,24 +2493,24 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -2515,222 +2520,222 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G3" t="s">
         <v>54</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>608</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>609</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>* [Digital Catapult](https://www.digicatapult.org.uk/)</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>616</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>617</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [ktn](https://ktn-uk.org/)</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>622</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [Innovate UK (part of UKRI)](https://www.gov.uk/government/organisations/innovate-uk)</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G6" t="s">
         <v>54</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [UK Research and Innovation (UKRI)](https://www.ukri.org/)</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [UKRI London Office](https://www.ukri.org/)</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [UKRI Bristol Office](https://www.ukri.org/)</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G9" t="s">
         <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>638</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>639</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>* [UK Business Angels](https://www.ukbaa.org.uk/)</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>641</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2743,19 +2748,19 @@
         <v>* [Level39](https://www.level39.co/)</v>
       </c>
       <c r="E11" t="s">
+        <v>470</v>
+      </c>
+      <c r="F11" t="s">
         <v>471</v>
-      </c>
-      <c r="F11" t="s">
-        <v>472</v>
       </c>
       <c r="G11"/>
       <c r="I11" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -2771,7 +2776,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G12"/>
     </row>
@@ -2800,34 +2805,34 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>456</v>
+      </c>
+      <c r="B14" t="s">
         <v>457</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>458</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>* [ConceptionX](https://conceptionx.org/)</v>
+      </c>
+      <c r="E14" t="s">
         <v>459</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="1"/>
-        <v>* [ConceptionX](https://conceptionx.org/)</v>
-      </c>
-      <c r="E14" t="s">
-        <v>460</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -2843,13 +2848,13 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -2862,10 +2867,10 @@
         <v>* [Cardiff Medicentre](http://www.cardiffmedicentre.co.uk/)</v>
       </c>
       <c r="E16" t="s">
+        <v>475</v>
+      </c>
+      <c r="F16" t="s">
         <v>476</v>
-      </c>
-      <c r="F16" t="s">
-        <v>477</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
@@ -2951,7 +2956,7 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -2973,7 +2978,7 @@
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G21"/>
     </row>
@@ -2993,7 +2998,7 @@
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G22" t="s">
         <v>43</v>
@@ -3015,7 +3020,7 @@
         <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>466</v>
       </c>
       <c r="G23" t="s">
         <v>47</v>
@@ -3037,7 +3042,7 @@
         <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G24" t="s">
         <v>49</v>
@@ -3056,7 +3061,7 @@
         <v>* [Seedcloud](https://www.seedcloud.com/)</v>
       </c>
       <c r="E25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F25" t="s">
         <v>55</v>
@@ -3081,7 +3086,7 @@
         <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G26" t="s">
         <v>58</v>
@@ -3100,10 +3105,10 @@
         <v>* [Seed Haus](https://thisisseedhaus.com/)</v>
       </c>
       <c r="E27" t="s">
+        <v>481</v>
+      </c>
+      <c r="F27" t="s">
         <v>482</v>
-      </c>
-      <c r="F27" t="s">
-        <v>483</v>
       </c>
       <c r="G27" t="s">
         <v>62</v>
@@ -3125,7 +3130,7 @@
         <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G28" t="s">
         <v>64</v>
@@ -3133,7 +3138,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
@@ -3146,10 +3151,10 @@
         <v>* [Imperial College White City Incubator](http://www.imperial.ac.uk/enterprise/business/incubator/)</v>
       </c>
       <c r="E29" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F29" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G29" t="s">
         <v>54</v>
@@ -3193,7 +3198,7 @@
         <v>76</v>
       </c>
       <c r="F31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G31"/>
     </row>
@@ -3213,7 +3218,7 @@
         <v>80</v>
       </c>
       <c r="F32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G32" t="s">
         <v>81</v>
@@ -3235,7 +3240,7 @@
         <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G33" t="s">
         <v>85</v>
@@ -3257,7 +3262,7 @@
         <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G34" t="s">
         <v>89</v>
@@ -3279,7 +3284,7 @@
         <v>92</v>
       </c>
       <c r="F35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G35" t="s">
         <v>54</v>
@@ -3301,7 +3306,7 @@
         <v>76</v>
       </c>
       <c r="F36" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G36" t="s">
         <v>95</v>
@@ -3323,7 +3328,7 @@
         <v>76</v>
       </c>
       <c r="F37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G37" t="s">
         <v>98</v>
@@ -3345,7 +3350,7 @@
         <v>76</v>
       </c>
       <c r="F38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G38" t="s">
         <v>101</v>
@@ -3367,7 +3372,7 @@
         <v>103</v>
       </c>
       <c r="F39" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G39" t="s">
         <v>54</v>
@@ -3389,7 +3394,7 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G40" t="s">
         <v>107</v>
@@ -3411,7 +3416,7 @@
         <v>111</v>
       </c>
       <c r="F41" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G41" t="s">
         <v>110</v>
@@ -3433,7 +3438,7 @@
         <v>111</v>
       </c>
       <c r="F42" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G42" t="s">
         <v>113</v>
@@ -3455,7 +3460,7 @@
         <v>117</v>
       </c>
       <c r="F43" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G43" t="s">
         <v>118</v>
@@ -3477,7 +3482,7 @@
         <v>111</v>
       </c>
       <c r="F44" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G44" t="s">
         <v>120</v>
@@ -3499,10 +3504,10 @@
         <v>124</v>
       </c>
       <c r="F45" t="s">
+        <v>489</v>
+      </c>
+      <c r="G45" t="s">
         <v>490</v>
-      </c>
-      <c r="G45" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3521,7 +3526,7 @@
         <v>126</v>
       </c>
       <c r="F46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G46" t="s">
         <v>128</v>
@@ -3543,7 +3548,7 @@
         <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G47" t="s">
         <v>131</v>
@@ -3565,7 +3570,7 @@
         <v>80</v>
       </c>
       <c r="F48" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G48" t="s">
         <v>135</v>
@@ -3587,7 +3592,7 @@
         <v>137</v>
       </c>
       <c r="F49" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G49" t="s">
         <v>139</v>
@@ -3609,7 +3614,7 @@
         <v>132</v>
       </c>
       <c r="F50" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G50" t="s">
         <v>142</v>
@@ -3629,7 +3634,7 @@
       </c>
       <c r="E51"/>
       <c r="F51" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G51"/>
     </row>
@@ -3649,7 +3654,7 @@
         <v>59</v>
       </c>
       <c r="F52" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G52" t="s">
         <v>147</v>
@@ -3657,7 +3662,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B53" t="s">
         <v>148</v>
@@ -3673,7 +3678,7 @@
         <v>132</v>
       </c>
       <c r="F53" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G53" t="s">
         <v>149</v>
@@ -3685,7 +3690,7 @@
         <v>151</v>
       </c>
       <c r="C54" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
@@ -3695,7 +3700,7 @@
         <v>76</v>
       </c>
       <c r="F54" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G54" t="s">
         <v>54</v>
@@ -3703,23 +3708,23 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>464</v>
+      </c>
+      <c r="B55" t="s">
+        <v>463</v>
+      </c>
+      <c r="C55" t="s">
+        <v>462</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>* [Oxford Accelerator](http://www.oxfordaccelerator.com/)</v>
+      </c>
+      <c r="E55" t="s">
         <v>465</v>
       </c>
-      <c r="B55" t="s">
-        <v>464</v>
-      </c>
-      <c r="C55" t="s">
-        <v>463</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>* [Oxford Accelerator](http://www.oxfordaccelerator.com/)</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>466</v>
-      </c>
-      <c r="F55" t="s">
-        <v>467</v>
       </c>
       <c r="G55" t="s">
         <v>54</v>
@@ -3741,7 +3746,7 @@
         <v>76</v>
       </c>
       <c r="F56" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G56" t="s">
         <v>154</v>
@@ -3762,7 +3767,9 @@
       <c r="E57" t="s">
         <v>156</v>
       </c>
-      <c r="F57"/>
+      <c r="F57" t="s">
+        <v>466</v>
+      </c>
       <c r="G57" t="s">
         <v>54</v>
       </c>
@@ -3783,7 +3790,7 @@
         <v>76</v>
       </c>
       <c r="F58" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G58" t="s">
         <v>160</v>
@@ -3805,7 +3812,7 @@
         <v>163</v>
       </c>
       <c r="F59" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G59" t="s">
         <v>54</v>
@@ -3847,7 +3854,7 @@
       </c>
       <c r="E61"/>
       <c r="F61" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G61" t="s">
         <v>170</v>
@@ -3869,7 +3876,7 @@
         <v>163</v>
       </c>
       <c r="F62" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G62" t="s">
         <v>173</v>
@@ -3891,7 +3898,7 @@
         <v>176</v>
       </c>
       <c r="F63" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G63" t="s">
         <v>54</v>
@@ -3913,7 +3920,7 @@
         <v>76</v>
       </c>
       <c r="F64" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G64" t="s">
         <v>179</v>
@@ -3935,7 +3942,7 @@
         <v>182</v>
       </c>
       <c r="F65" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G65" t="s">
         <v>54</v>
@@ -3955,7 +3962,7 @@
       </c>
       <c r="E66"/>
       <c r="F66" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G66" t="s">
         <v>185</v>
@@ -3977,7 +3984,7 @@
         <v>176</v>
       </c>
       <c r="F67" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G67" t="s">
         <v>54</v>
@@ -3999,7 +4006,7 @@
         <v>163</v>
       </c>
       <c r="F68" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G68" t="s">
         <v>190</v>
@@ -4021,7 +4028,7 @@
         <v>163</v>
       </c>
       <c r="F69" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G69" t="s">
         <v>193</v>
@@ -4043,7 +4050,7 @@
         <v>197</v>
       </c>
       <c r="F70" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G70" t="s">
         <v>196</v>
@@ -4087,7 +4094,7 @@
         <v>76</v>
       </c>
       <c r="F72" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G72" t="s">
         <v>203</v>
@@ -4109,7 +4116,7 @@
         <v>163</v>
       </c>
       <c r="F73" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G73" t="s">
         <v>206</v>
@@ -4131,7 +4138,7 @@
         <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G74" t="s">
         <v>209</v>
@@ -4153,7 +4160,7 @@
         <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G75" t="s">
         <v>212</v>
@@ -4197,7 +4204,7 @@
         <v>73</v>
       </c>
       <c r="F77" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G77" t="s">
         <v>218</v>
@@ -4219,7 +4226,7 @@
         <v>163</v>
       </c>
       <c r="F78" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G78" t="s">
         <v>221</v>
@@ -4263,7 +4270,7 @@
         <v>163</v>
       </c>
       <c r="F80" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G80" t="s">
         <v>228</v>
@@ -4285,7 +4292,7 @@
         <v>182</v>
       </c>
       <c r="F81" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G81" t="s">
         <v>54</v>
@@ -4307,7 +4314,7 @@
         <v>234</v>
       </c>
       <c r="F82" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G82" t="s">
         <v>233</v>
@@ -4329,7 +4336,7 @@
         <v>73</v>
       </c>
       <c r="F83" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G83" t="s">
         <v>54</v>
@@ -4351,7 +4358,7 @@
         <v>163</v>
       </c>
       <c r="F84" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G84" t="s">
         <v>238</v>
@@ -4373,7 +4380,7 @@
         <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G85" t="s">
         <v>241</v>
@@ -4395,7 +4402,7 @@
         <v>156</v>
       </c>
       <c r="F86" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G86" t="s">
         <v>54</v>
@@ -4417,7 +4424,7 @@
         <v>156</v>
       </c>
       <c r="F87" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G87" t="s">
         <v>54</v>
@@ -4439,7 +4446,7 @@
         <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G88" t="s">
         <v>249</v>
@@ -4461,7 +4468,7 @@
         <v>253</v>
       </c>
       <c r="F89" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G89" t="s">
         <v>252</v>
@@ -4483,7 +4490,7 @@
         <v>73</v>
       </c>
       <c r="F90" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G90" t="s">
         <v>256</v>
@@ -4505,7 +4512,7 @@
         <v>73</v>
       </c>
       <c r="F91" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G91" t="s">
         <v>259</v>
@@ -4527,7 +4534,7 @@
         <v>73</v>
       </c>
       <c r="F92" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G92" t="s">
         <v>261</v>
@@ -4549,7 +4556,7 @@
         <v>73</v>
       </c>
       <c r="F93" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G93" t="s">
         <v>54</v>
@@ -4571,7 +4578,7 @@
         <v>73</v>
       </c>
       <c r="F94" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G94" t="s">
         <v>267</v>
@@ -4615,7 +4622,7 @@
         <v>272</v>
       </c>
       <c r="F96" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G96" t="s">
         <v>275</v>
@@ -4637,7 +4644,7 @@
         <v>279</v>
       </c>
       <c r="F97" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G97" t="s">
         <v>278</v>
@@ -4659,7 +4666,7 @@
         <v>73</v>
       </c>
       <c r="F98" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G98" t="s">
         <v>282</v>
@@ -4681,7 +4688,7 @@
         <v>182</v>
       </c>
       <c r="F99" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G99" t="s">
         <v>285</v>
@@ -4703,10 +4710,10 @@
         <v>163</v>
       </c>
       <c r="F100" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G100" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -4725,7 +4732,7 @@
         <v>73</v>
       </c>
       <c r="F101" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G101" t="s">
         <v>290</v>
@@ -4747,7 +4754,7 @@
         <v>73</v>
       </c>
       <c r="F102" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G102" t="s">
         <v>293</v>
@@ -4769,7 +4776,7 @@
         <v>73</v>
       </c>
       <c r="F103" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G103" t="s">
         <v>296</v>
@@ -4791,7 +4798,7 @@
         <v>73</v>
       </c>
       <c r="F104" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G104" t="s">
         <v>299</v>
@@ -4813,41 +4820,41 @@
         <v>36</v>
       </c>
       <c r="F105" t="s">
+        <v>658</v>
+      </c>
+      <c r="G105" t="s">
         <v>302</v>
-      </c>
-      <c r="G105" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106"/>
       <c r="B106" t="s">
+        <v>303</v>
+      </c>
+      <c r="C106" t="s">
         <v>304</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="str">
+        <f t="shared" si="2"/>
+        <v>* [The Nova Centre](https://www.keele.ac.uk/business/scienceandinnovationpark/)</v>
+      </c>
+      <c r="E106" t="s">
         <v>305</v>
       </c>
-      <c r="D106" t="str">
-        <f t="shared" si="2"/>
-        <v>* [The Nova Centre](https://www.keele.ac.uk/business/scienceandinnovationpark/)</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
+        <v>517</v>
+      </c>
+      <c r="G106" t="s">
         <v>306</v>
-      </c>
-      <c r="F106" t="s">
-        <v>518</v>
-      </c>
-      <c r="G106" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107"/>
       <c r="B107" t="s">
+        <v>307</v>
+      </c>
+      <c r="C107" t="s">
         <v>308</v>
-      </c>
-      <c r="C107" t="s">
-        <v>309</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
@@ -4857,41 +4864,41 @@
         <v>126</v>
       </c>
       <c r="F107" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108"/>
       <c r="B108" t="s">
+        <v>310</v>
+      </c>
+      <c r="C108" t="s">
         <v>311</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Witney Business &amp; Innovation Centre](https://www.witney-bic.co.uk/)</v>
+      </c>
+      <c r="E108" t="s">
+        <v>318</v>
+      </c>
+      <c r="F108" t="s">
+        <v>518</v>
+      </c>
+      <c r="G108" t="s">
         <v>312</v>
-      </c>
-      <c r="D108" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Witney Business &amp; Innovation Centre](https://www.witney-bic.co.uk/)</v>
-      </c>
-      <c r="E108" t="s">
-        <v>319</v>
-      </c>
-      <c r="F108" t="s">
-        <v>519</v>
-      </c>
-      <c r="G108" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109"/>
       <c r="B109" t="s">
+        <v>313</v>
+      </c>
+      <c r="C109" t="s">
         <v>314</v>
-      </c>
-      <c r="C109" t="s">
-        <v>315</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
@@ -4901,7 +4908,7 @@
         <v>73</v>
       </c>
       <c r="F109" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G109" t="s">
         <v>54</v>
@@ -4910,32 +4917,32 @@
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110"/>
       <c r="B110" t="s">
+        <v>315</v>
+      </c>
+      <c r="C110" t="s">
         <v>316</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="str">
+        <f t="shared" si="2"/>
+        <v>* [BU Student Incubation Centre (BUSI)](https://www.hugedomains.com/domain_profile.cfm?d=bucfe&amp;e=com)</v>
+      </c>
+      <c r="E110" t="s">
+        <v>318</v>
+      </c>
+      <c r="F110" t="s">
+        <v>519</v>
+      </c>
+      <c r="G110" t="s">
         <v>317</v>
-      </c>
-      <c r="D110" t="str">
-        <f t="shared" si="2"/>
-        <v>* [BU Student Incubation Centre (BUSI)](https://www.hugedomains.com/domain_profile.cfm?d=bucfe&amp;e=com)</v>
-      </c>
-      <c r="E110" t="s">
-        <v>319</v>
-      </c>
-      <c r="F110" t="s">
-        <v>520</v>
-      </c>
-      <c r="G110" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111"/>
       <c r="B111" t="s">
+        <v>319</v>
+      </c>
+      <c r="C111" t="s">
         <v>320</v>
-      </c>
-      <c r="C111" t="s">
-        <v>321</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
@@ -4945,7 +4952,7 @@
         <v>73</v>
       </c>
       <c r="F111" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G111" t="s">
         <v>54</v>
@@ -4954,10 +4961,10 @@
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112"/>
       <c r="B112" t="s">
+        <v>321</v>
+      </c>
+      <c r="C112" t="s">
         <v>322</v>
-      </c>
-      <c r="C112" t="s">
-        <v>323</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
@@ -4967,7 +4974,7 @@
         <v>73</v>
       </c>
       <c r="F112" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G112" t="s">
         <v>54</v>
@@ -4976,32 +4983,32 @@
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113"/>
       <c r="B113" t="s">
+        <v>323</v>
+      </c>
+      <c r="C113" t="s">
         <v>324</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Live Lab](https://www.livelab.co.uk/)</v>
+      </c>
+      <c r="E113" t="s">
+        <v>326</v>
+      </c>
+      <c r="F113" t="s">
+        <v>579</v>
+      </c>
+      <c r="G113" t="s">
         <v>325</v>
-      </c>
-      <c r="D113" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Live Lab](https://www.livelab.co.uk/)</v>
-      </c>
-      <c r="E113" t="s">
-        <v>327</v>
-      </c>
-      <c r="F113" t="s">
-        <v>580</v>
-      </c>
-      <c r="G113" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114"/>
       <c r="B114" t="s">
+        <v>327</v>
+      </c>
+      <c r="C114" t="s">
         <v>328</v>
-      </c>
-      <c r="C114" t="s">
-        <v>329</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
@@ -5011,19 +5018,19 @@
         <v>59</v>
       </c>
       <c r="F114" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G114" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115"/>
       <c r="B115" t="s">
+        <v>330</v>
+      </c>
+      <c r="C115" t="s">
         <v>331</v>
-      </c>
-      <c r="C115" t="s">
-        <v>332</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
@@ -5031,19 +5038,19 @@
       </c>
       <c r="E115"/>
       <c r="F115" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G115" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116"/>
       <c r="B116" t="s">
+        <v>333</v>
+      </c>
+      <c r="C116" t="s">
         <v>334</v>
-      </c>
-      <c r="C116" t="s">
-        <v>335</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
@@ -5053,19 +5060,19 @@
         <v>8</v>
       </c>
       <c r="F116" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117"/>
       <c r="B117" t="s">
+        <v>336</v>
+      </c>
+      <c r="C117" t="s">
         <v>337</v>
-      </c>
-      <c r="C117" t="s">
-        <v>338</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
@@ -5075,19 +5082,19 @@
         <v>73</v>
       </c>
       <c r="F117" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G117" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118"/>
       <c r="B118" t="s">
+        <v>339</v>
+      </c>
+      <c r="C118" t="s">
         <v>340</v>
-      </c>
-      <c r="C118" t="s">
-        <v>341</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
@@ -5097,7 +5104,7 @@
         <v>73</v>
       </c>
       <c r="F118" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G118" t="s">
         <v>54</v>
@@ -5106,10 +5113,10 @@
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119"/>
       <c r="B119" t="s">
+        <v>341</v>
+      </c>
+      <c r="C119" t="s">
         <v>342</v>
-      </c>
-      <c r="C119" t="s">
-        <v>343</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
@@ -5117,63 +5124,63 @@
       </c>
       <c r="E119"/>
       <c r="F119" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G119" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120"/>
       <c r="B120" t="s">
+        <v>344</v>
+      </c>
+      <c r="C120" t="s">
         <v>345</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Momentum Business Incubator](http://www.worcesterenterprise.org/incubator-support-package/)</v>
+      </c>
+      <c r="E120" t="s">
+        <v>525</v>
+      </c>
+      <c r="F120" t="s">
+        <v>526</v>
+      </c>
+      <c r="G120" t="s">
         <v>346</v>
-      </c>
-      <c r="D120" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Momentum Business Incubator](http://www.worcesterenterprise.org/incubator-support-package/)</v>
-      </c>
-      <c r="E120" t="s">
-        <v>526</v>
-      </c>
-      <c r="F120" t="s">
-        <v>527</v>
-      </c>
-      <c r="G120" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121"/>
       <c r="B121" t="s">
+        <v>347</v>
+      </c>
+      <c r="C121" t="s">
         <v>348</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="str">
+        <f t="shared" si="2"/>
+        <v>* [NoWFOOD Centre](https://www1.chester.ac.uk/business-growth/nowfood)</v>
+      </c>
+      <c r="E121" t="s">
         <v>349</v>
       </c>
-      <c r="D121" t="str">
-        <f t="shared" si="2"/>
-        <v>* [NoWFOOD Centre](https://www1.chester.ac.uk/business-growth/nowfood)</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
+        <v>582</v>
+      </c>
+      <c r="G121" t="s">
         <v>350</v>
-      </c>
-      <c r="F121" t="s">
-        <v>583</v>
-      </c>
-      <c r="G121" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122"/>
       <c r="B122" t="s">
+        <v>351</v>
+      </c>
+      <c r="C122" t="s">
         <v>352</v>
-      </c>
-      <c r="C122" t="s">
-        <v>353</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
@@ -5183,19 +5190,19 @@
         <v>76</v>
       </c>
       <c r="F122" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G122" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123"/>
       <c r="B123" t="s">
+        <v>354</v>
+      </c>
+      <c r="C123" t="s">
         <v>355</v>
-      </c>
-      <c r="C123" t="s">
-        <v>356</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
@@ -5203,38 +5210,38 @@
       </c>
       <c r="E123"/>
       <c r="F123" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G123" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124"/>
       <c r="B124" t="s">
+        <v>357</v>
+      </c>
+      <c r="C124" t="s">
         <v>358</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UHatch](https://www.gcu.ac.uk/uhatch/)</v>
+      </c>
+      <c r="E124" t="s">
+        <v>360</v>
+      </c>
+      <c r="F124" t="s">
+        <v>585</v>
+      </c>
+      <c r="G124" t="s">
         <v>359</v>
-      </c>
-      <c r="D124" t="str">
-        <f t="shared" si="2"/>
-        <v>* [UHatch](https://www.gcu.ac.uk/uhatch/)</v>
-      </c>
-      <c r="E124" t="s">
-        <v>361</v>
-      </c>
-      <c r="F124" t="s">
-        <v>586</v>
-      </c>
-      <c r="G124" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125"/>
       <c r="B125" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C125" t="s">
         <v>21</v>
@@ -5247,93 +5254,93 @@
         <v>21</v>
       </c>
       <c r="F125" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G125"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126"/>
       <c r="B126" t="s">
+        <v>362</v>
+      </c>
+      <c r="C126" t="s">
         <v>363</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Fareham Innovation Centre](https://www.fareham-ic.co.uk/)</v>
+      </c>
+      <c r="E126" t="s">
         <v>364</v>
       </c>
-      <c r="D126" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Fareham Innovation Centre](https://www.fareham-ic.co.uk/)</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="F126" t="s">
+        <v>586</v>
+      </c>
+      <c r="G126" t="s">
         <v>365</v>
-      </c>
-      <c r="F126" t="s">
-        <v>587</v>
-      </c>
-      <c r="G126" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127"/>
       <c r="B127" t="s">
+        <v>366</v>
+      </c>
+      <c r="C127" t="s">
         <v>367</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="str">
+        <f t="shared" si="2"/>
+        <v>* [High Growth Centre](https://www1.chester.ac.uk/business-growth/thornton-science-park)</v>
+      </c>
+      <c r="E127" t="s">
         <v>368</v>
       </c>
-      <c r="D127" t="str">
-        <f t="shared" si="2"/>
-        <v>* [High Growth Centre](https://www1.chester.ac.uk/business-growth/thornton-science-park)</v>
-      </c>
-      <c r="E127" t="s">
-        <v>369</v>
-      </c>
       <c r="F127" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G127" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128"/>
       <c r="B128" t="s">
+        <v>369</v>
+      </c>
+      <c r="C128" t="s">
         <v>370</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Ideas Factory Incubation Centre](https://www.nua.ac.uk/for-business/incubation-centre-facility-hire/)</v>
+      </c>
+      <c r="E128" t="s">
+        <v>372</v>
+      </c>
+      <c r="F128" t="s">
+        <v>587</v>
+      </c>
+      <c r="G128" t="s">
         <v>371</v>
-      </c>
-      <c r="D128" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Ideas Factory Incubation Centre](https://www.nua.ac.uk/for-business/incubation-centre-facility-hire/)</v>
-      </c>
-      <c r="E128" t="s">
-        <v>373</v>
-      </c>
-      <c r="F128" t="s">
-        <v>588</v>
-      </c>
-      <c r="G128" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129"/>
       <c r="B129" t="s">
+        <v>373</v>
+      </c>
+      <c r="C129" t="s">
         <v>374</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="str">
+        <f t="shared" si="2"/>
+        <v>* [InTechnology Enterprise incubator](https://www.leeds.ac.uk/news/article/3668/young_entrepreneurs_get_a_chance_to_shine)</v>
+      </c>
+      <c r="E129" t="s">
         <v>375</v>
       </c>
-      <c r="D129" t="str">
-        <f t="shared" si="2"/>
-        <v>* [InTechnology Enterprise incubator](https://www.leeds.ac.uk/news/article/3668/young_entrepreneurs_get_a_chance_to_shine)</v>
-      </c>
-      <c r="E129" t="s">
-        <v>376</v>
-      </c>
       <c r="F129" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G129" t="s">
         <v>54</v>
@@ -5342,32 +5349,32 @@
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130"/>
       <c r="B130" t="s">
+        <v>376</v>
+      </c>
+      <c r="C130" t="s">
         <v>377</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="str">
+        <f t="shared" si="2"/>
+        <v>* [Marine Robotics Innovation Centre Hub](https://noc-innovations.co.uk/marine-robotics-innovation-centre)</v>
+      </c>
+      <c r="E130" t="s">
         <v>378</v>
       </c>
-      <c r="D130" t="str">
-        <f t="shared" si="2"/>
-        <v>* [Marine Robotics Innovation Centre Hub](https://noc-innovations.co.uk/marine-robotics-innovation-centre)</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="F130" t="s">
+        <v>529</v>
+      </c>
+      <c r="G130" t="s">
         <v>379</v>
-      </c>
-      <c r="F130" t="s">
-        <v>530</v>
-      </c>
-      <c r="G130" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131"/>
       <c r="B131" t="s">
+        <v>380</v>
+      </c>
+      <c r="C131" t="s">
         <v>381</v>
-      </c>
-      <c r="C131" t="s">
-        <v>382</v>
       </c>
       <c r="D131" t="str">
         <f t="shared" si="2"/>
@@ -5375,95 +5382,95 @@
       </c>
       <c r="E131"/>
       <c r="F131" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G131" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132"/>
       <c r="B132" t="s">
+        <v>383</v>
+      </c>
+      <c r="C132" t="s">
         <v>384</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="str">
+        <f t="shared" si="2"/>
+        <v>* [The BioHub Birmingham](https://www.birminghamresearchpark.co.uk/biohub/)</v>
+      </c>
+      <c r="E132" t="s">
         <v>385</v>
       </c>
-      <c r="D132" t="str">
-        <f t="shared" si="2"/>
-        <v>* [The BioHub Birmingham](https://www.birminghamresearchpark.co.uk/biohub/)</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="F132" t="s">
+        <v>588</v>
+      </c>
+      <c r="G132" t="s">
         <v>386</v>
-      </c>
-      <c r="F132" t="s">
-        <v>589</v>
-      </c>
-      <c r="G132" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133"/>
       <c r="B133" t="s">
+        <v>387</v>
+      </c>
+      <c r="C133" t="s">
         <v>388</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="str">
+        <f t="shared" si="2"/>
+        <v>* [The Ingenuity Lab](https://www.nottingham.ac.uk/business/businesscentres/hgi/ingenuity-lab/about-the-ingenuity-lab.aspx)</v>
+      </c>
+      <c r="E133" t="s">
+        <v>390</v>
+      </c>
+      <c r="F133" t="s">
+        <v>589</v>
+      </c>
+      <c r="G133" t="s">
         <v>389</v>
-      </c>
-      <c r="D133" t="str">
-        <f t="shared" si="2"/>
-        <v>* [The Ingenuity Lab](https://www.nottingham.ac.uk/business/businesscentres/hgi/ingenuity-lab/about-the-ingenuity-lab.aspx)</v>
-      </c>
-      <c r="E133" t="s">
-        <v>391</v>
-      </c>
-      <c r="F133" t="s">
-        <v>590</v>
-      </c>
-      <c r="G133" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134"/>
       <c r="B134" t="s">
+        <v>391</v>
+      </c>
+      <c r="C134" t="s">
+        <v>394</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="2"/>
+        <v>* [UBC Leeds Digital Hub](https://leeds.tech/workspace/the-digital-hub/)</v>
+      </c>
+      <c r="E134" t="s">
+        <v>395</v>
+      </c>
+      <c r="F134" t="s">
         <v>392</v>
       </c>
-      <c r="C134" t="s">
-        <v>395</v>
-      </c>
-      <c r="D134" t="str">
-        <f t="shared" si="2"/>
-        <v>* [UBC Leeds Digital Hub](https://leeds.tech/workspace/the-digital-hub/)</v>
-      </c>
-      <c r="E134" t="s">
-        <v>396</v>
-      </c>
-      <c r="F134" t="s">
+      <c r="G134" t="s">
         <v>393</v>
-      </c>
-      <c r="G134" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135"/>
       <c r="B135" t="s">
+        <v>396</v>
+      </c>
+      <c r="C135" t="s">
         <v>397</v>
       </c>
-      <c r="C135" t="s">
-        <v>398</v>
-      </c>
       <c r="D135" t="str">
         <f t="shared" si="2"/>
         <v>* [WB100](http://wosskowbrownfoundation.org.uk/)</v>
       </c>
       <c r="E135" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F135" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G135" t="s">
         <v>54</v>
@@ -5472,20 +5479,20 @@
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136"/>
       <c r="B136" t="s">
+        <v>398</v>
+      </c>
+      <c r="C136" t="s">
         <v>399</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="str">
+        <f t="shared" si="2"/>
+        <v>* [BioData Innovation Centre](https://www.sanger.ac.uk/about/campus)</v>
+      </c>
+      <c r="E136" t="s">
         <v>400</v>
       </c>
-      <c r="D136" t="str">
-        <f t="shared" si="2"/>
-        <v>* [BioData Innovation Centre](https://www.sanger.ac.uk/about/campus)</v>
-      </c>
-      <c r="E136" t="s">
-        <v>401</v>
-      </c>
       <c r="F136" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G136" t="s">
         <v>54</v>
@@ -5494,32 +5501,32 @@
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137"/>
       <c r="B137" t="s">
+        <v>401</v>
+      </c>
+      <c r="C137" t="s">
         <v>402</v>
       </c>
-      <c r="C137" t="s">
-        <v>403</v>
-      </c>
       <c r="D137" t="str">
         <f t="shared" si="2"/>
         <v>* [Canopy Exeter](https://www.exetersciencepark.co.uk/)</v>
       </c>
       <c r="E137" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F137" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G137" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138"/>
       <c r="B138" t="s">
+        <v>403</v>
+      </c>
+      <c r="C138" t="s">
         <v>404</v>
-      </c>
-      <c r="C138" t="s">
-        <v>405</v>
       </c>
       <c r="D138" t="str">
         <f t="shared" si="2"/>
@@ -5529,107 +5536,107 @@
         <v>8</v>
       </c>
       <c r="F138" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G138" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139"/>
       <c r="B139" t="s">
+        <v>406</v>
+      </c>
+      <c r="C139" t="s">
         <v>407</v>
-      </c>
-      <c r="C139" t="s">
-        <v>408</v>
       </c>
       <c r="D139" t="str">
         <f t="shared" ref="D139:D156" si="3">CONCATENATE("* [",B139,"](",C139,")")</f>
         <v>* [Londoneast](https://www.londoneast-uk.com/)</v>
       </c>
       <c r="E139" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F139" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G139" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140"/>
       <c r="B140" t="s">
+        <v>410</v>
+      </c>
+      <c r="C140" t="s">
         <v>411</v>
-      </c>
-      <c r="C140" t="s">
-        <v>412</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="3"/>
         <v>* [North East Space Incubation Programme](https://www.northeasttechnologypark.com/)</v>
       </c>
       <c r="E140" t="s">
+        <v>412</v>
+      </c>
+      <c r="F140" t="s">
+        <v>593</v>
+      </c>
+      <c r="G140" t="s">
         <v>413</v>
-      </c>
-      <c r="F140" t="s">
-        <v>594</v>
-      </c>
-      <c r="G140" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141"/>
       <c r="B141" t="s">
+        <v>414</v>
+      </c>
+      <c r="C141" t="s">
         <v>415</v>
-      </c>
-      <c r="C141" t="s">
-        <v>416</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="3"/>
         <v>* [OpTIC Space Industry Incubation Programme](http://www.glyndwrinnovations.co.uk/incubation/)</v>
       </c>
       <c r="E141" t="s">
+        <v>416</v>
+      </c>
+      <c r="F141" t="s">
+        <v>594</v>
+      </c>
+      <c r="G141" t="s">
         <v>417</v>
-      </c>
-      <c r="F141" t="s">
-        <v>595</v>
-      </c>
-      <c r="G141" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142"/>
       <c r="B142" t="s">
+        <v>418</v>
+      </c>
+      <c r="C142" t="s">
         <v>419</v>
-      </c>
-      <c r="C142" t="s">
-        <v>420</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="3"/>
         <v>* [Roslin Innovation Centre](https://www.roslininnovationcentre.com/)</v>
       </c>
       <c r="E142" t="s">
+        <v>420</v>
+      </c>
+      <c r="F142" t="s">
+        <v>595</v>
+      </c>
+      <c r="G142" t="s">
         <v>421</v>
-      </c>
-      <c r="F142" t="s">
-        <v>596</v>
-      </c>
-      <c r="G142" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143"/>
       <c r="B143" t="s">
+        <v>422</v>
+      </c>
+      <c r="C143" t="s">
         <v>423</v>
-      </c>
-      <c r="C143" t="s">
-        <v>424</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="3"/>
@@ -5639,16 +5646,16 @@
         <v>21</v>
       </c>
       <c r="F143" t="s">
-        <v>21</v>
+        <v>466</v>
       </c>
       <c r="G143" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144"/>
       <c r="B144" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C144" t="s">
         <v>18</v>
@@ -5658,10 +5665,10 @@
         <v>* [Space Incubator](https://www.lusep.co.uk/)</v>
       </c>
       <c r="E144" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F144" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G144" t="s">
         <v>54</v>
@@ -5670,10 +5677,10 @@
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145"/>
       <c r="B145" t="s">
+        <v>426</v>
+      </c>
+      <c r="C145" t="s">
         <v>427</v>
-      </c>
-      <c r="C145" t="s">
-        <v>428</v>
       </c>
       <c r="D145" t="str">
         <f t="shared" si="3"/>
@@ -5683,7 +5690,7 @@
         <v>8</v>
       </c>
       <c r="F145" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G145" t="s">
         <v>54</v>
@@ -5692,64 +5699,64 @@
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146"/>
       <c r="B146" t="s">
+        <v>428</v>
+      </c>
+      <c r="C146" t="s">
         <v>429</v>
-      </c>
-      <c r="C146" t="s">
-        <v>430</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="3"/>
         <v>* [Ashton Old Baths Innovation Centre](https://www.ashtonoldbaths.co.uk/)</v>
       </c>
       <c r="E146" t="s">
+        <v>430</v>
+      </c>
+      <c r="F146" t="s">
+        <v>535</v>
+      </c>
+      <c r="G146" t="s">
         <v>431</v>
-      </c>
-      <c r="F146" t="s">
-        <v>536</v>
-      </c>
-      <c r="G146" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147"/>
       <c r="B147" t="s">
+        <v>432</v>
+      </c>
+      <c r="C147" t="s">
         <v>433</v>
-      </c>
-      <c r="C147" t="s">
-        <v>434</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="3"/>
         <v>* [Aurora Cambridge](https://www.bas.ac.uk/science/science-and-innovation/aurora-cambridge/)</v>
       </c>
       <c r="E147" t="s">
+        <v>434</v>
+      </c>
+      <c r="F147" t="s">
+        <v>596</v>
+      </c>
+      <c r="G147" t="s">
         <v>435</v>
-      </c>
-      <c r="F147" t="s">
-        <v>597</v>
-      </c>
-      <c r="G147" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148"/>
       <c r="B148" t="s">
+        <v>436</v>
+      </c>
+      <c r="C148" t="s">
         <v>437</v>
-      </c>
-      <c r="C148" t="s">
-        <v>438</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="3"/>
         <v>* [Charnwood Campus](http://charnwoodcampus.com/)</v>
       </c>
       <c r="E148" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F148" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G148" t="s">
         <v>54</v>
@@ -5758,20 +5765,20 @@
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149"/>
       <c r="B149" t="s">
+        <v>438</v>
+      </c>
+      <c r="C149" t="s">
         <v>439</v>
-      </c>
-      <c r="C149" t="s">
-        <v>440</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="3"/>
         <v>* [The Spot Hive](https://www.sportingchanceinitiative.co.uk/the-sport-hive)</v>
       </c>
       <c r="E149" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F149" t="s">
-        <v>21</v>
+        <v>466</v>
       </c>
       <c r="G149" t="s">
         <v>54</v>
@@ -5780,20 +5787,20 @@
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150"/>
       <c r="B150" t="s">
+        <v>441</v>
+      </c>
+      <c r="C150" t="s">
         <v>442</v>
-      </c>
-      <c r="C150" t="s">
-        <v>443</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="3"/>
         <v>* [STEAMHouse](https://www.bcu.ac.uk/business/steam/steamhouse)</v>
       </c>
       <c r="E150" t="s">
+        <v>598</v>
+      </c>
+      <c r="F150" t="s">
         <v>599</v>
-      </c>
-      <c r="F150" t="s">
-        <v>600</v>
       </c>
       <c r="G150" t="s">
         <v>54</v>
@@ -5802,10 +5809,10 @@
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151"/>
       <c r="B151" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C151" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="3"/>
@@ -5815,7 +5822,7 @@
         <v>156</v>
       </c>
       <c r="F151" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G151" t="s">
         <v>54</v>
@@ -5824,20 +5831,20 @@
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152"/>
       <c r="B152" t="s">
+        <v>445</v>
+      </c>
+      <c r="C152" t="s">
         <v>446</v>
-      </c>
-      <c r="C152" t="s">
-        <v>447</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="3"/>
         <v>* [UNIT DX](https://sciencecreates.co.uk/)</v>
       </c>
       <c r="E152" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F152" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G152" t="s">
         <v>54</v>
@@ -5846,20 +5853,20 @@
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153"/>
       <c r="B153" t="s">
+        <v>448</v>
+      </c>
+      <c r="C153" t="s">
         <v>449</v>
-      </c>
-      <c r="C153" t="s">
-        <v>450</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="3"/>
         <v>* [Guildhall Creative Entrepreneurs](https://www.gsmd.ac.uk/youth_adult_learning/creative_business_support/guildhall_creative_entrepreneurs/)</v>
       </c>
       <c r="E153" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F153" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G153" t="s">
         <v>54</v>
@@ -5868,20 +5875,20 @@
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154"/>
       <c r="B154" t="s">
+        <v>451</v>
+      </c>
+      <c r="C154" t="s">
         <v>452</v>
-      </c>
-      <c r="C154" t="s">
-        <v>453</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="3"/>
         <v>* [C11 Cyber Security and Digital Centre](https://www.glos.ac.uk/business-and-partnerships/c11-cyber-security-and-digital-innovation-centre/)</v>
       </c>
       <c r="E154" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F154" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G154" t="s">
         <v>54</v>
@@ -5890,10 +5897,10 @@
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155"/>
       <c r="B155" t="s">
+        <v>454</v>
+      </c>
+      <c r="C155" t="s">
         <v>455</v>
-      </c>
-      <c r="C155" t="s">
-        <v>456</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="3"/>
@@ -5903,7 +5910,7 @@
         <v>73</v>
       </c>
       <c r="F155" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G155" t="s">
         <v>54</v>
@@ -5911,32 +5918,32 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D156" s="2" t="str">
         <f t="shared" si="3"/>
         <v>* [Founders Institute London](https://fi.co/overview)</v>
       </c>
       <c r="E156" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F156" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="G156" t="s">
         <v>54</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -5961,32 +5968,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0D6E3D-312B-D943-BFDE-8DF8AE29187A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>656</v>
+      </c>
+      <c r="C2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>